<commit_message>
combinging all our stuff
</commit_message>
<xml_diff>
--- a/Products Excel Sheet.xlsx
+++ b/Products Excel Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\aminsakib360\CSC 322 Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06ECA18F-D1B7-4370-B5AF-EF3A9F707D69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F9A9804-0599-4EEC-8974-DBC138898D09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29700" yWindow="990" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{306CB091-4AB8-49AB-A91B-D8F3334D4B83}"/>
+    <workbookView xWindow="31485" yWindow="840" windowWidth="21600" windowHeight="11385" activeTab="7" xr2:uid="{306CB091-4AB8-49AB-A91B-D8F3334D4B83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="182">
   <si>
     <t>CPU:</t>
   </si>
@@ -1954,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE4F49C-A739-40BD-874D-F2F2F1ABE8A8}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,7 +2198,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,7 +2334,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2490,10 +2491,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38BFABF-981E-4691-8123-5908D8B0D238}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,7 +2502,7 @@
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>164</v>
       </c>
@@ -2520,8 +2521,11 @@
       <c r="G1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>168</v>
       </c>
@@ -2537,8 +2541,11 @@
       <c r="G2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>172</v>
       </c>
@@ -2554,8 +2561,11 @@
       <c r="G3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>174</v>
       </c>
@@ -2571,8 +2581,11 @@
       <c r="G4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>177</v>
       </c>
@@ -2587,6 +2600,9 @@
       </c>
       <c r="G5" t="s">
         <v>180</v>
+      </c>
+      <c r="H5">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>